<commit_message>
Extension of the model to 2070 for additional outputs (add-outputs)
BDbDT: Extended by forecast.ets
FoHObDT:
- Census Projections extended by forcast.ets in 5 yr increments as was done previously
- Projections: Extension of previous functions through to 2070
HOIpTP: Extension of existing trend function
SCoC: Click & Drag basic pattern extension of source data, corresponding formulas extended
VoaSL: No need to extend, single value
</commit_message>
<xml_diff>
--- a/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
+++ b/InputData/add-outputs/BDbDT/BAU Deaths by Demographic Trait.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ssy02/Desktop/Brazil/eps-brazil-3.4.1/InputData/add-outputs/BDbDT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anima\OneDrive\Desktop\Models\eps-brazil-cpl2\InputData\add-outputs\BDbDT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8517D57A-3336-0243-B28B-D987C0D1172F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B77FF4-104D-442E-B06D-02001A83104F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34200" windowHeight="21380" activeTab="2" xr2:uid="{07D21EFD-220B-4C60-85BD-FCD4C246A818}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="2" xr2:uid="{07D21EFD-220B-4C60-85BD-FCD4C246A818}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -544,21 +544,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66936CFD-0A84-4062-AAF5-5F189C33D342}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="81.5" customWidth="1"/>
+    <col min="2" max="2" width="81.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -566,48 +566,48 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B5" s="18" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" s="2"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -633,14 +633,14 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="3" width="12.6640625" style="9" customWidth="1"/>
     <col min="4" max="29" width="12.6640625" style="8" customWidth="1"/>
     <col min="30" max="36" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B2" s="17" t="s">
         <v>14</v>
       </c>
@@ -747,7 +747,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B3" s="13" t="s">
         <v>13</v>
       </c>
@@ -882,7 +882,7 @@
         <v>1653228.1364885506</v>
       </c>
     </row>
-    <row r="4" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B4" s="13" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>900222.48160388088</v>
       </c>
     </row>
-    <row r="5" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B5" s="13" t="s">
         <v>6</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>751525.3534900879</v>
       </c>
     </row>
-    <row r="6" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:36" x14ac:dyDescent="0.45">
       <c r="B6" s="13" t="s">
         <v>15</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G8" s="8" t="s">
         <v>17</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="AH8" s="6"/>
       <c r="AI8" s="6"/>
     </row>
-    <row r="9" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G9" s="8" t="s">
         <v>16</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="AI9" s="7"/>
       <c r="AJ9" s="4"/>
     </row>
-    <row r="10" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G10" s="10" t="s">
         <v>18</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="11" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G11" s="11" t="s">
         <v>13</v>
       </c>
@@ -1539,7 +1539,7 @@
         <v>1.0842752829768336</v>
       </c>
     </row>
-    <row r="12" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G12" s="11" t="s">
         <v>5</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>1.0791459611002661</v>
       </c>
     </row>
-    <row r="13" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G13" s="11" t="s">
         <v>6</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>1.0891782286053451</v>
       </c>
     </row>
-    <row r="14" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G14" s="11"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9"/>
@@ -1792,7 +1792,7 @@
       <c r="AH14" s="8"/>
       <c r="AI14" s="8"/>
     </row>
-    <row r="15" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G15" s="12" t="s">
         <v>13</v>
       </c>
@@ -1884,7 +1884,7 @@
         <v>232933276</v>
       </c>
     </row>
-    <row r="16" spans="2:36" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:36" x14ac:dyDescent="0.45">
       <c r="G16" s="12" t="s">
         <v>5</v>
       </c>
@@ -1976,7 +1976,7 @@
         <v>113300060</v>
       </c>
     </row>
-    <row r="17" spans="7:36" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:36" x14ac:dyDescent="0.45">
       <c r="G17" s="12" t="s">
         <v>6</v>
       </c>
@@ -2082,19 +2082,19 @@
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AZ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="32" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.46484375" customWidth="1"/>
+    <col min="2" max="32" width="10.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" x14ac:dyDescent="0.45">
       <c r="B1">
         <v>2020</v>
       </c>
@@ -2188,8 +2188,68 @@
       <c r="AF1">
         <v>2050</v>
       </c>
+      <c r="AG1">
+        <v>2051</v>
+      </c>
+      <c r="AH1">
+        <v>2052</v>
+      </c>
+      <c r="AI1">
+        <v>2053</v>
+      </c>
+      <c r="AJ1">
+        <v>2054</v>
+      </c>
+      <c r="AK1">
+        <v>2055</v>
+      </c>
+      <c r="AL1">
+        <v>2056</v>
+      </c>
+      <c r="AM1">
+        <v>2057</v>
+      </c>
+      <c r="AN1">
+        <v>2058</v>
+      </c>
+      <c r="AO1">
+        <v>2059</v>
+      </c>
+      <c r="AP1">
+        <v>2060</v>
+      </c>
+      <c r="AQ1">
+        <v>2061</v>
+      </c>
+      <c r="AR1">
+        <v>2062</v>
+      </c>
+      <c r="AS1">
+        <v>2063</v>
+      </c>
+      <c r="AT1">
+        <v>2064</v>
+      </c>
+      <c r="AU1">
+        <v>2065</v>
+      </c>
+      <c r="AV1">
+        <v>2066</v>
+      </c>
+      <c r="AW1">
+        <v>2067</v>
+      </c>
+      <c r="AX1">
+        <v>2068</v>
+      </c>
+      <c r="AY1">
+        <v>2069</v>
+      </c>
+      <c r="AZ1">
+        <v>2070</v>
+      </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2317,8 +2377,88 @@
         <f>IBGE!AJ4</f>
         <v>900222.48160388088</v>
       </c>
+      <c r="AG2">
+        <f>_xlfn.FORECAST.ETS(AG1,$B$2:$AF$2,$B$1:$AF$1)</f>
+        <v>903654.23163187306</v>
+      </c>
+      <c r="AH2">
+        <f t="shared" ref="AH2:AZ2" si="0">_xlfn.FORECAST.ETS(AH1,$B$2:$AF$2,$B$1:$AF$1)</f>
+        <v>905270.87842702924</v>
+      </c>
+      <c r="AI2">
+        <f t="shared" si="0"/>
+        <v>906887.5252221853</v>
+      </c>
+      <c r="AJ2">
+        <f t="shared" si="0"/>
+        <v>908504.17201734148</v>
+      </c>
+      <c r="AK2">
+        <f t="shared" si="0"/>
+        <v>910120.81881249754</v>
+      </c>
+      <c r="AL2">
+        <f t="shared" si="0"/>
+        <v>911737.4656076536</v>
+      </c>
+      <c r="AM2">
+        <f t="shared" si="0"/>
+        <v>913354.11240280978</v>
+      </c>
+      <c r="AN2">
+        <f t="shared" si="0"/>
+        <v>914970.75919796585</v>
+      </c>
+      <c r="AO2">
+        <f t="shared" si="0"/>
+        <v>916587.40599312203</v>
+      </c>
+      <c r="AP2">
+        <f t="shared" si="0"/>
+        <v>918204.05278827809</v>
+      </c>
+      <c r="AQ2">
+        <f t="shared" si="0"/>
+        <v>919820.69958343415</v>
+      </c>
+      <c r="AR2">
+        <f t="shared" si="0"/>
+        <v>921437.34637859033</v>
+      </c>
+      <c r="AS2">
+        <f t="shared" si="0"/>
+        <v>923053.99317374639</v>
+      </c>
+      <c r="AT2">
+        <f t="shared" si="0"/>
+        <v>924670.63996890257</v>
+      </c>
+      <c r="AU2">
+        <f t="shared" si="0"/>
+        <v>926287.28676405863</v>
+      </c>
+      <c r="AV2">
+        <f t="shared" si="0"/>
+        <v>927903.9335592147</v>
+      </c>
+      <c r="AW2">
+        <f t="shared" si="0"/>
+        <v>929520.58035437088</v>
+      </c>
+      <c r="AX2">
+        <f t="shared" si="0"/>
+        <v>931137.22714952694</v>
+      </c>
+      <c r="AY2">
+        <f t="shared" si="0"/>
+        <v>932753.87394468312</v>
+      </c>
+      <c r="AZ2">
+        <f t="shared" si="0"/>
+        <v>934370.52073983918</v>
+      </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2446,8 +2586,88 @@
         <f>IBGE!AJ5</f>
         <v>751525.3534900879</v>
       </c>
+      <c r="AG3">
+        <f>_xlfn.FORECAST.ETS(AG1,$B$3:$AF$3,$B$1:$AF$1)</f>
+        <v>758819.12106273707</v>
+      </c>
+      <c r="AH3">
+        <f t="shared" ref="AH3:AZ3" si="1">_xlfn.FORECAST.ETS(AH1,$B$3:$AF$3,$B$1:$AF$1)</f>
+        <v>760731.83537665207</v>
+      </c>
+      <c r="AI3">
+        <f t="shared" si="1"/>
+        <v>762644.54969056719</v>
+      </c>
+      <c r="AJ3">
+        <f t="shared" si="1"/>
+        <v>764557.26400448231</v>
+      </c>
+      <c r="AK3">
+        <f t="shared" si="1"/>
+        <v>766469.9783183973</v>
+      </c>
+      <c r="AL3">
+        <f t="shared" si="1"/>
+        <v>768382.69263231242</v>
+      </c>
+      <c r="AM3">
+        <f t="shared" si="1"/>
+        <v>770295.40694622754</v>
+      </c>
+      <c r="AN3">
+        <f t="shared" si="1"/>
+        <v>772208.12126014254</v>
+      </c>
+      <c r="AO3">
+        <f t="shared" si="1"/>
+        <v>774120.83557405765</v>
+      </c>
+      <c r="AP3">
+        <f t="shared" si="1"/>
+        <v>776033.54988797277</v>
+      </c>
+      <c r="AQ3">
+        <f t="shared" si="1"/>
+        <v>777946.26420188777</v>
+      </c>
+      <c r="AR3">
+        <f t="shared" si="1"/>
+        <v>779858.97851580288</v>
+      </c>
+      <c r="AS3">
+        <f t="shared" si="1"/>
+        <v>781771.692829718</v>
+      </c>
+      <c r="AT3">
+        <f t="shared" si="1"/>
+        <v>783684.407143633</v>
+      </c>
+      <c r="AU3">
+        <f t="shared" si="1"/>
+        <v>785597.12145754811</v>
+      </c>
+      <c r="AV3">
+        <f t="shared" si="1"/>
+        <v>787509.83577146323</v>
+      </c>
+      <c r="AW3">
+        <f t="shared" si="1"/>
+        <v>789422.55008537823</v>
+      </c>
+      <c r="AX3">
+        <f t="shared" si="1"/>
+        <v>791335.26439929334</v>
+      </c>
+      <c r="AY3">
+        <f t="shared" si="1"/>
+        <v>793247.97871320834</v>
+      </c>
+      <c r="AZ3">
+        <f t="shared" si="1"/>
+        <v>795160.69302712346</v>
+      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2544,8 +2764,68 @@
       <c r="AF4" s="20">
         <v>0</v>
       </c>
+      <c r="AG4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2642,8 +2922,68 @@
       <c r="AF5" s="20">
         <v>0</v>
       </c>
+      <c r="AG5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2740,8 +3080,68 @@
       <c r="AF6" s="20">
         <v>0</v>
       </c>
+      <c r="AG6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2838,8 +3238,68 @@
       <c r="AF7" s="20">
         <v>0</v>
       </c>
+      <c r="AG7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2936,8 +3396,68 @@
       <c r="AF8" s="20">
         <v>0</v>
       </c>
+      <c r="AG8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="20">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -3032,6 +3552,66 @@
         <v>0</v>
       </c>
       <c r="AF9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="20">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="20">
         <v>0</v>
       </c>
     </row>

</xml_diff>